<commit_message>
add:se agrega artista al sistema
</commit_message>
<xml_diff>
--- a/reportes/asistencia/ReporteAsistenciaMarzo2025.xlsx
+++ b/reportes/asistencia/ReporteAsistenciaMarzo2025.xlsx
@@ -122,6 +122,24 @@
     <t>31</t>
   </si>
   <si>
+    <t>Lucas Alonso</t>
+  </si>
+  <si>
+    <t>3050</t>
+  </si>
+  <si>
+    <t>50697897</t>
+  </si>
+  <si>
+    <t>Discontinuo</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>P.M</t>
+  </si>
+  <si>
     <t>José Fernandéz</t>
   </si>
   <si>
@@ -131,28 +149,10 @@
     <t>45607907</t>
   </si>
   <si>
-    <t>Discontinuo</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>P.T</t>
   </si>
   <si>
     <t>P</t>
-  </si>
-  <si>
-    <t>Lucas Alonso</t>
-  </si>
-  <si>
-    <t>3050</t>
-  </si>
-  <si>
-    <t>50697897</t>
-  </si>
-  <si>
-    <t>P.M</t>
   </si>
   <si>
     <t>REFERENCIAS:   |   P: Presente (Dos turnos)   |   P.M: Presente horario de mañana   |   P.T: Presente horario de tarde   |   A: Ausente   |   F/C: Franco compensatorio   |   LAR: Licencia Anual Reglamentaria   |   C/M: Certificado Médico   |   L/E: Licencia por Estudio</t>
@@ -468,13 +468,13 @@
         <v>40</v>
       </c>
       <c r="R3" t="s" s="2">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S3" t="s" s="2">
         <v>41</v>
       </c>
       <c r="T3" t="s" s="2">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="U3" t="s" s="2">
         <v>40</v>
@@ -524,13 +524,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s" s="2">
         <v>43</v>
       </c>
-      <c r="B4" t="s" s="2">
+      <c r="C4" t="s" s="2">
         <v>44</v>
-      </c>
-      <c r="C4" t="s" s="2">
-        <v>45</v>
       </c>
       <c r="D4" t="s" s="2">
         <v>39</v>
@@ -575,13 +575,13 @@
         <v>40</v>
       </c>
       <c r="R4" t="s" s="2">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="S4" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T4" t="s" s="2">
         <v>46</v>
-      </c>
-      <c r="T4" t="s" s="2">
-        <v>40</v>
       </c>
       <c r="U4" t="s" s="2">
         <v>40</v>

</xml_diff>